<commit_message>
Modified a xml entry
</commit_message>
<xml_diff>
--- a/WS2012R2/lisa/docs/VSS testcases.xlsx
+++ b/WS2012R2/lisa/docs/VSS testcases.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr date1904="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="2600" yWindow="560" windowWidth="20440" windowHeight="19620"/>
   </bookViews>
   <sheets>
-    <sheet name="VSS" sheetId="1" r:id="rId4"/>
+    <sheet name="VSS" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
   <si>
     <t>Tescase</t>
   </si>
@@ -51,7 +58,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -118,7 +125,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -183,7 +190,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -251,7 +258,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -346,7 +353,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -363,7 +370,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -421,7 +428,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -438,7 +445,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -488,7 +495,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -505,7 +512,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -574,7 +581,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -591,7 +598,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -704,7 +711,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -830,7 +837,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -901,7 +908,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -961,20 +968,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
     </font>
     <font>
       <sz val="10"/>
@@ -982,21 +981,16 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1056,45 +1050,51 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1102,29 +1102,80 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffff5f5d"/>
-      <rgbColor rgb="ff9ce159"/>
-      <rgbColor rgb="fff4f4f4"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFFF5F5D"/>
+      <rgbColor rgb="FF9CE159"/>
+      <rgbColor rgb="FFF4F4F4"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -1316,7 +1367,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1325,7 +1376,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1334,7 +1385,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1343,7 +1394,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1352,7 +1403,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1361,7 +1412,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1473,8 +1524,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -1482,14 +1533,14 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1508,7 +1559,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1516,7 +1567,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -1544,7 +1595,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1570,7 +1621,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1596,7 +1647,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1622,7 +1673,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1648,7 +1699,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1674,7 +1725,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1700,7 +1751,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1726,7 +1777,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1752,7 +1803,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1765,9 +1816,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1783,7 +1840,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1802,7 +1859,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1828,7 +1885,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1854,7 +1911,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1880,7 +1937,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1906,7 +1963,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1932,7 +1989,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1958,7 +2015,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1984,7 +2041,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2010,7 +2067,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2036,7 +2093,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2049,9 +2106,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -2064,7 +2127,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2083,7 +2146,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2113,7 +2176,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2139,7 +2202,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2165,7 +2228,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2191,7 +2254,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2217,7 +2280,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2243,7 +2306,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2269,7 +2332,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2295,7 +2358,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2321,7 +2384,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2334,500 +2397,509 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:IV19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5391" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="39.375" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.55469" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.7734" style="1" customWidth="1"/>
-    <col min="7" max="7" width="49.1641" style="1" customWidth="1"/>
-    <col min="8" max="8" width="45.0938" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="49.125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="45.125" style="1" customWidth="1"/>
     <col min="9" max="256" width="6.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.55" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:8" ht="20.5" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="188.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:8" ht="188.5" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s" s="5">
+      <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s" s="5">
+      <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s" s="5">
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" ht="188.35" customHeight="1">
-      <c r="A3" t="s" s="7">
+    <row r="3" spans="1:8" ht="188.25" customHeight="1">
+      <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s" s="8">
+      <c r="B3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s" s="9">
+      <c r="C3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s" s="9">
+      <c r="D3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s" s="9">
+      <c r="E3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s" s="9">
+      <c r="F3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s" s="9">
+      <c r="G3" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" ht="188.35" customHeight="1">
-      <c r="A4" t="s" s="7">
+    <row r="4" spans="1:8" ht="188.25" customHeight="1">
+      <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s" s="5">
+      <c r="C4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s" s="5">
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s" s="5">
+      <c r="E4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s" s="5">
+      <c r="F4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s" s="5">
+      <c r="G4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" ht="116.35" customHeight="1">
-      <c r="A5" t="s" s="7">
+    <row r="5" spans="1:8" ht="116.25" customHeight="1">
+      <c r="A5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s" s="8">
+      <c r="B5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s" s="9">
+      <c r="C5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s" s="9">
+      <c r="D5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s" s="9">
+      <c r="E5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s" s="9">
+      <c r="F5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" ht="188.35" customHeight="1">
-      <c r="A6" t="s" s="7">
+    <row r="6" spans="1:8" ht="188.25" customHeight="1">
+      <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s" s="5">
+      <c r="C6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s" s="5">
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s" s="5">
+      <c r="E6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s" s="5">
+      <c r="F6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G6" t="s" s="5">
+      <c r="G6" s="5" t="s">
         <v>31</v>
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" ht="128.35" customHeight="1">
-      <c r="A7" t="s" s="7">
+    <row r="7" spans="1:8" ht="128.25" customHeight="1">
+      <c r="A7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s" s="8">
+      <c r="B7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s" s="9">
+      <c r="C7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D7" t="s" s="9">
+      <c r="D7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E7" t="s" s="9">
+      <c r="E7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F7" t="s" s="9">
+      <c r="F7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G7" t="s" s="9">
+      <c r="G7" s="9" t="s">
         <v>37</v>
       </c>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" ht="140.35" customHeight="1">
-      <c r="A8" t="s" s="7">
+    <row r="8" spans="1:8" ht="140.25" customHeight="1">
+      <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B8" t="s" s="4">
+      <c r="B8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s" s="5">
+      <c r="C8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D8" t="s" s="5">
+      <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="s" s="5">
+      <c r="E8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s" s="5">
+      <c r="F8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G8" t="s" s="5">
+      <c r="G8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H8" t="s" s="5">
+      <c r="H8" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" ht="140.35" customHeight="1">
-      <c r="A9" t="s" s="7">
+    <row r="9" spans="1:8" ht="140.25" customHeight="1">
+      <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B9" t="s" s="8">
+      <c r="B9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C9" t="s" s="9">
+      <c r="C9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D9" t="s" s="9">
+      <c r="D9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" t="s" s="9">
+      <c r="E9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" t="s" s="9">
+      <c r="F9" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G9" t="s" s="9">
+      <c r="G9" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="9"/>
+      <c r="H9" s="13"/>
     </row>
-    <row r="10" ht="210.6" customHeight="1">
-      <c r="A10" t="s" s="7">
+    <row r="10" spans="1:8" ht="210.5" customHeight="1">
+      <c r="A10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B10" t="s" s="4">
+      <c r="B10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C10" t="s" s="5">
+      <c r="C10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D10" t="s" s="5">
+      <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E10" t="s" s="5">
+      <c r="E10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F10" t="s" s="5">
+      <c r="F10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G10" t="s" s="5">
+      <c r="G10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H10" t="s" s="5">
+      <c r="H10" s="12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" ht="253.7" customHeight="1">
-      <c r="A11" t="s" s="7">
+    <row r="11" spans="1:8" ht="253.75" customHeight="1">
+      <c r="A11" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B11" t="s" s="8">
+      <c r="B11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C11" t="s" s="9">
+      <c r="C11" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D11" t="s" s="9">
+      <c r="D11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E11" t="s" s="9">
+      <c r="E11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F11" t="s" s="9">
+      <c r="F11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G11" t="s" s="9">
+      <c r="G11" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="9"/>
+      <c r="H11" s="13"/>
     </row>
-    <row r="12" ht="140.35" customHeight="1">
-      <c r="A12" t="s" s="7">
+    <row r="12" spans="1:8" ht="140.25" customHeight="1">
+      <c r="A12" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B12" t="s" s="4">
+      <c r="B12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C12" t="s" s="5">
+      <c r="C12" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D12" t="s" s="5">
+      <c r="D12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E12" t="s" s="5">
+      <c r="E12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F12" t="s" s="5">
+      <c r="F12" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G12" t="s" s="5">
+      <c r="G12" s="5" t="s">
         <v>61</v>
       </c>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" ht="128.35" customHeight="1">
-      <c r="A13" t="s" s="7">
+    <row r="13" spans="1:8" ht="128.25" customHeight="1">
+      <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B13" t="s" s="8">
+      <c r="B13" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C13" t="s" s="9">
+      <c r="C13" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D13" t="s" s="9">
+      <c r="D13" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E13" t="s" s="9">
+      <c r="E13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F13" t="s" s="9">
+      <c r="F13" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="G13" t="s" s="9">
+      <c r="G13" s="9" t="s">
         <v>67</v>
       </c>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" ht="152.35" customHeight="1">
-      <c r="A14" t="s" s="3">
+    <row r="14" spans="1:8" ht="152.25" customHeight="1">
+      <c r="A14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B14" t="s" s="4">
+      <c r="B14" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C14" t="s" s="5">
+      <c r="C14" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D14" t="s" s="5">
+      <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E14" t="s" s="5">
+      <c r="E14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F14" t="s" s="5">
+      <c r="F14" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G14" t="s" s="5">
+      <c r="G14" s="5" t="s">
         <v>72</v>
       </c>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" ht="140.35" customHeight="1">
-      <c r="A15" t="s" s="7">
+    <row r="15" spans="1:8" ht="140.25" customHeight="1">
+      <c r="A15" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B15" t="s" s="8">
+      <c r="B15" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C15" t="s" s="9">
+      <c r="C15" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D15" t="s" s="9">
+      <c r="D15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E15" t="s" s="9">
+      <c r="E15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F15" t="s" s="9">
+      <c r="F15" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G15" t="s" s="9">
+      <c r="G15" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="H15" t="s" s="9">
+      <c r="H15" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" ht="140.35" customHeight="1">
-      <c r="A16" t="s" s="7">
+    <row r="16" spans="1:8" ht="140.25" customHeight="1">
+      <c r="A16" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B16" t="s" s="4">
+      <c r="B16" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C16" t="s" s="5">
+      <c r="C16" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D16" t="s" s="5">
+      <c r="D16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E16" t="s" s="5">
+      <c r="E16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F16" t="s" s="5">
+      <c r="F16" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G16" t="s" s="5">
+      <c r="G16" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H16" t="s" s="5">
+      <c r="H16" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" ht="176.35" customHeight="1">
-      <c r="A17" t="s" s="3">
+    <row r="17" spans="1:8" ht="176.25" customHeight="1">
+      <c r="A17" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B17" t="s" s="8">
+      <c r="B17" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C17" t="s" s="9">
+      <c r="C17" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D17" t="s" s="9">
+      <c r="D17" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E17" t="s" s="9">
+      <c r="E17" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F17" t="s" s="9">
+      <c r="F17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G17" t="s" s="9">
+      <c r="G17" s="9" t="s">
         <v>89</v>
       </c>
       <c r="H17" s="10"/>
     </row>
-    <row r="18" ht="44.35" customHeight="1">
-      <c r="A18" t="s" s="7">
+    <row r="18" spans="1:8" ht="44.25" customHeight="1">
+      <c r="A18" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B18" t="s" s="4">
+      <c r="B18" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C18" t="s" s="5">
+      <c r="C18" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D18" t="s" s="5">
+      <c r="D18" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E18" t="s" s="5">
+      <c r="E18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F18" t="s" s="5">
+      <c r="F18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G18" t="s" s="5">
+      <c r="G18" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H18" t="s" s="5">
+      <c r="H18" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="19" ht="128.35" customHeight="1">
-      <c r="A19" t="s" s="3">
+    <row r="19" spans="1:8" ht="128.25" customHeight="1">
+      <c r="A19" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B19" t="s" s="8">
+      <c r="B19" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C19" t="s" s="9">
+      <c r="C19" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D19" t="s" s="9">
+      <c r="D19" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E19" t="s" s="9">
+      <c r="E19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F19" t="s" s="9">
+      <c r="F19" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="G19" t="s" s="9">
+      <c r="G19" s="9" t="s">
         <v>101</v>
       </c>
       <c r="H19" s="10"/>
@@ -2838,9 +2910,14 @@
     <mergeCell ref="H8:H9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update to the VSS testcases description
</commit_message>
<xml_diff>
--- a/WS2012R2/lisa/docs/VSS testcases.xlsx
+++ b/WS2012R2/lisa/docs/VSS testcases.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="560" windowWidth="20440" windowHeight="19620"/>
+    <workbookView xWindow="2600" yWindow="560" windowWidth="36160" windowHeight="23340"/>
   </bookViews>
   <sheets>
     <sheet name="VSS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -534,19 +534,6 @@
 3. Perform Backup. 
 4. Perform Restore. 
 5. Check boot message (/var/log/boot.msg) for any recovering journal error.</t>
-  </si>
-  <si>
-    <t>&lt;test&gt;
-&lt;testName&gt;VSS_BackupRestore_CSV_VHDX&lt;/testName&gt;
-   	&lt;testScript&gt;setupscripts\VSS_BackupRestore_Partition.ps1&lt;/testScript&gt; 
-	&lt;testParams&gt;
-		&lt;param&gt;driveletter=F:&lt;/param&gt;
-		&lt;param&gt;FILESYS=ext4&lt;/param&gt;
-		&lt;param&gt;TC_COVERED=VSS-09&lt;/param&gt;
-	&lt;/testParams&gt;
-	&lt;timeout&gt;1200&lt;/timeout&gt;
-	&lt;OnError&gt;Continue&lt;/OnError&gt;
-&lt;/test&gt;</t>
   </si>
   <si>
     <t>SMB Backup Configuration(Only On Window8 Server)
@@ -615,20 +602,6 @@
     </r>
   </si>
   <si>
-    <t>&lt;test&gt;
-&lt;testName&gt;VSS_BackupRestore_CSV_VHD&lt;/testName&gt;
-   	&lt;testScript&gt;setupscripts\VSS_BackupRestore_Partition.ps1&lt;/testScript&gt; 
-	&lt;testParams&gt;
-		&lt;param&gt;driveletter=F:&lt;/param&gt;
-		&lt;param&gt;FILESYS=ext4&lt;/param&gt;
-		&lt;param&gt;TC_COVERED=VSS-10&lt;/param&gt;
-	&lt;/testParams&gt;
-	&lt;cleanupScript&gt;setupscripts\RemoveHardDisk.ps1&lt;/cleanupScript&gt;
-	&lt;timeout&gt;1200&lt;/timeout&gt;
-	&lt;OnError&gt;Continue&lt;/OnError&gt;
-&lt;/test&gt;</t>
-  </si>
-  <si>
     <t>VSS-11</t>
   </si>
   <si>
@@ -964,12 +937,39 @@
 	&lt;OnERROR&gt;Continue&lt;/OnERROR&gt;
 &lt;/test&gt;</t>
   </si>
+  <si>
+    <t>&lt;test&gt;
+&lt;testName&gt;VSS_BackupRestore_SMB_VHDX&lt;/testName&gt;
+   	&lt;testScript&gt;setupscripts\VSS_BackupRestore_Partition.ps1&lt;/testScript&gt; 
+	&lt;testParams&gt;
+		&lt;param&gt;driveletter=F:&lt;/param&gt;
+		&lt;param&gt;FILESYS=ext4&lt;/param&gt;
+		&lt;param&gt;TC_COVERED=VSS-09&lt;/param&gt;
+	&lt;/testParams&gt;
+	&lt;timeout&gt;1200&lt;/timeout&gt;
+	&lt;OnError&gt;Continue&lt;/OnError&gt;
+&lt;/test&gt;</t>
+  </si>
+  <si>
+    <t>&lt;test&gt;
+&lt;testName&gt;VSS_BackupRestore_SMB_VHD&lt;/testName&gt;
+   	&lt;testScript&gt;setupscripts\VSS_BackupRestore_Partition.ps1&lt;/testScript&gt; 
+	&lt;testParams&gt;
+		&lt;param&gt;driveletter=F:&lt;/param&gt;
+		&lt;param&gt;FILESYS=ext4&lt;/param&gt;
+		&lt;param&gt;TC_COVERED=VSS-10&lt;/param&gt;
+	&lt;/testParams&gt;
+	&lt;cleanupScript&gt;setupscripts\RemoveHardDisk.ps1&lt;/cleanupScript&gt;
+	&lt;timeout&gt;1200&lt;/timeout&gt;
+	&lt;OnError&gt;Continue&lt;/OnError&gt;
+&lt;/test&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -991,6 +991,18 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1049,8 +1061,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
@@ -1098,7 +1116,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2421,8 +2441,8 @@
   </sheetPr>
   <dimension ref="A1:IV19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -2676,18 +2696,18 @@
         <v>41</v>
       </c>
       <c r="G10" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="253.75" customHeight="1">
       <c r="A11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>50</v>
@@ -2702,67 +2722,67 @@
         <v>41</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:8" ht="140.25" customHeight="1">
       <c r="A12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" ht="128.25" customHeight="1">
       <c r="A13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="D13" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>65</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" ht="152.25" customHeight="1">
       <c r="A14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>11</v>
@@ -2771,22 +2791,22 @@
         <v>12</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" ht="140.25" customHeight="1">
       <c r="A15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>11</v>
@@ -2795,24 +2815,24 @@
         <v>18</v>
       </c>
       <c r="F15" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="140.25" customHeight="1">
       <c r="A16" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>11</v>
@@ -2821,27 +2841,27 @@
         <v>18</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="176.25" customHeight="1">
       <c r="A17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="D17" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>12</v>
@@ -2850,22 +2870,22 @@
         <v>13</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8" ht="44.25" customHeight="1">
       <c r="A18" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>18</v>
@@ -2874,33 +2894,33 @@
         <v>36</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="128.25" customHeight="1">
       <c r="A19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="D19" s="9" t="s">
         <v>97</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>99</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H19" s="10"/>
     </row>

</xml_diff>

<commit_message>
Fixed the VSS fail testcase
</commit_message>
<xml_diff>
--- a/WS2012R2/lisa/docs/VSS testcases.xlsx
+++ b/WS2012R2/lisa/docs/VSS testcases.xlsx
@@ -922,22 +922,6 @@
     <t>1. Guest should not panic / call trace in case of backup/restore failure</t>
   </si>
   <si>
-    <t>VSS_BackupRestore_Fail.ps1
-VSS_Disk_Fail.sh</t>
-  </si>
-  <si>
-    <t>&lt;test&gt;
-&lt;testName&gt;VSS_BackupRestore_Fail&lt;/testName&gt;
-	&lt;testScript&gt;setupscripts\VSS_BackupRestore_Fail.ps1&lt;/testScript&gt; 
-	&lt;testParams&gt;
-		&lt;param&gt;driveletter=F:&lt;/param&gt;
-		&lt;param&gt;TC_COVERED=VSS-18&lt;/param&gt;
-	&lt;/testParams&gt;
-	&lt;timeout&gt;1200&lt;/timeout&gt;
-	&lt;OnERROR&gt;Continue&lt;/OnERROR&gt;
-&lt;/test&gt;</t>
-  </si>
-  <si>
     <t>&lt;test&gt;
 &lt;testName&gt;VSS_BackupRestore_SMB_VHDX&lt;/testName&gt;
    	&lt;testScript&gt;setupscripts\VSS_BackupRestore_Partition.ps1&lt;/testScript&gt; 
@@ -963,6 +947,28 @@
 	&lt;timeout&gt;1200&lt;/timeout&gt;
 	&lt;OnError&gt;Continue&lt;/OnError&gt;
 &lt;/test&gt;</t>
+  </si>
+  <si>
+    <t>AddHardDisk.ps1
+VSS_BackupRestore_Fail.ps1
+VSS_Disk_Fail.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;test&gt;
+    &lt;testName&gt;VSS_BackupRestore_Fail&lt;/testName&gt;
+        &lt;setupScript&gt;setupscripts\AddHardDisk.ps1&lt;/setupScript&gt;
+        &lt;testScript&gt;setupscripts\VSS_BackupRestore_Fail.ps1&lt;/testScript&gt; 
+        &lt;testParams&gt;
+            &lt;param&gt;driveletter=F:&lt;/param&gt;
+            &lt;param&gt;SCSI=0,1,Dynamic&lt;/param&gt;
+            &lt;param&gt;IDE=0,1,Dynamic&lt;/param&gt;
+            &lt;param&gt;FILESYS-ext3&lt;/param&gt;
+            &lt;param&gt;TC_COVERED=VSS-18&lt;/param&gt;
+        &lt;/testParams&gt;
+        &lt;cleanupScript&gt;setupscripts\RemoveHardDisk.ps1&lt;/cleanupScript&gt;
+        &lt;timeout&gt;1200&lt;/timeout&gt;
+        &lt;OnERROR&gt;Continue&lt;/OnERROR&gt;
+    &lt;/test&gt;</t>
   </si>
 </sst>
 </file>
@@ -2441,8 +2447,8 @@
   </sheetPr>
   <dimension ref="A1:IV19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -2696,7 +2702,7 @@
         <v>41</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>51</v>
@@ -2722,7 +2728,7 @@
         <v>41</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H11" s="13"/>
     </row>
@@ -2917,10 +2923,10 @@
         <v>12</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H19" s="10"/>
     </row>

</xml_diff>